<commit_message>
Updated Gantt Chart Trial (Singh)
</commit_message>
<xml_diff>
--- a/COE127L_DOE_Grp6_Gantt.xlsx
+++ b/COE127L_DOE_Grp6_Gantt.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COE127L-B1-18\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COE127L-B1-16\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="570" windowWidth="21600" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="570" windowWidth="19200" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -36,92 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>ACTIVITY</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Corbel"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Complete</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Actual (beyond plan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Corbel"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Corbel"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Complete (beyond plan)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve"> Period Highlight:</t>
   </si>
   <si>
@@ -204,13 +123,46 @@
   </si>
   <si>
     <t>Gathering of results (Test)</t>
+  </si>
+  <si>
+    <t>Justine Estoesta</t>
+  </si>
+  <si>
+    <t>Uploading of initial files</t>
+  </si>
+  <si>
+    <t>Estoesta, Omaña, Singh</t>
+  </si>
+  <si>
+    <t>Patricia Omaña</t>
+  </si>
+  <si>
+    <t>Estoesta, Singh</t>
+  </si>
+  <si>
+    <t>Winci John Singh</t>
+  </si>
+  <si>
+    <t>Omaña, Singh</t>
+  </si>
+  <si>
+    <t>Estoesta, Omaña</t>
+  </si>
+  <si>
+    <t>% Complete</t>
+  </si>
+  <si>
+    <t>Actual (beyond plan)</t>
+  </si>
+  <si>
+    <t>% Complete (beyond plan)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -240,23 +192,6 @@
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1" tint="0.24994659260841701"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="7"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1" tint="0.24994659260841701"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -305,41 +240,38 @@
       <scheme val="major"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="14"/>
       <color theme="1" tint="0.24994659260841701"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1" tint="0.24994659260841701"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="14"/>
+      <color theme="7"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="7"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="14"/>
       <color theme="1" tint="0.24994659260841701"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="7"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1" tint="0.24994659260841701"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="major"/>
+      <sz val="14"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -475,14 +407,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" applyFill="0" applyProtection="0">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="2" applyFill="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -491,44 +423,44 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFill="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFill="0" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFill="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="6" borderId="1">
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -538,125 +470,110 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="3">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="6">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="7">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="8" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="6" borderId="1" xfId="13">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="7" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="6" borderId="1" xfId="13" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="14" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="14" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="15" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="16" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="16" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="17" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="18" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="18" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="11">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="9" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="11" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="8" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="2" xfId="3" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1067,535 +984,1244 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AW32"/>
+  <dimension ref="A1:AW33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="K11" sqref="B11:K11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="68" zoomScaleNormal="68" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="2" customWidth="1"/>
-    <col min="3" max="6" width="11.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.25" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.75" style="1"/>
+    <col min="1" max="1" width="53.625" customWidth="1"/>
+    <col min="2" max="2" width="27.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.25" style="3" customWidth="1"/>
+    <col min="8" max="8" width="4.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="3.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="26" width="4.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="29" max="37" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="39" max="47" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="5.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:49" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="1:49" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+    </row>
+    <row r="2" spans="1:49" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11">
+        <v>36</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB2" s="21"/>
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="21"/>
+      <c r="AG2" s="22"/>
+      <c r="AH2" s="23"/>
+      <c r="AI2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17"/>
+      <c r="AL2" s="17"/>
+      <c r="AM2" s="17"/>
+      <c r="AN2" s="17"/>
+      <c r="AO2" s="17"/>
+      <c r="AP2" s="17"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+    </row>
+    <row r="3" spans="1:49" s="4" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="29"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="30"/>
+      <c r="U3" s="30"/>
+      <c r="V3" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="30"/>
+      <c r="Z3" s="30"/>
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK3" s="24"/>
+      <c r="AL3" s="24"/>
+      <c r="AM3" s="24"/>
+      <c r="AN3" s="24"/>
+      <c r="AO3" s="24"/>
+      <c r="AP3" s="24"/>
+      <c r="AQ3" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR3" s="24"/>
+      <c r="AS3" s="24"/>
+      <c r="AT3" s="24"/>
+      <c r="AU3" s="24"/>
+      <c r="AV3" s="24"/>
+      <c r="AW3" s="24"/>
+    </row>
+    <row r="4" spans="1:49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33">
+        <v>1</v>
+      </c>
+      <c r="I4" s="33">
+        <v>2</v>
+      </c>
+      <c r="J4" s="33">
+        <v>3</v>
+      </c>
+      <c r="K4" s="33">
+        <v>4</v>
+      </c>
+      <c r="L4" s="33">
+        <v>5</v>
+      </c>
+      <c r="M4" s="33">
+        <v>6</v>
+      </c>
+      <c r="N4" s="33">
+        <v>7</v>
+      </c>
+      <c r="O4" s="33">
+        <v>8</v>
+      </c>
+      <c r="P4" s="33">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="33">
+        <v>10</v>
+      </c>
+      <c r="R4" s="33">
+        <v>11</v>
+      </c>
+      <c r="S4" s="33">
+        <v>12</v>
+      </c>
+      <c r="T4" s="33">
+        <v>13</v>
+      </c>
+      <c r="U4" s="33">
+        <v>14</v>
+      </c>
+      <c r="V4" s="33">
+        <v>15</v>
+      </c>
+      <c r="W4" s="33">
+        <v>16</v>
+      </c>
+      <c r="X4" s="33">
+        <v>17</v>
+      </c>
+      <c r="Y4" s="33">
+        <v>18</v>
+      </c>
+      <c r="Z4" s="33">
+        <v>19</v>
+      </c>
+      <c r="AA4" s="33">
+        <v>20</v>
+      </c>
+      <c r="AB4" s="33">
         <v>21</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="2:49" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="5" t="s">
+      <c r="AC4" s="33">
+        <v>22</v>
+      </c>
+      <c r="AD4" s="33">
+        <v>23</v>
+      </c>
+      <c r="AE4" s="33">
+        <v>24</v>
+      </c>
+      <c r="AF4" s="33">
+        <v>25</v>
+      </c>
+      <c r="AG4" s="33">
+        <v>26</v>
+      </c>
+      <c r="AH4" s="33">
+        <v>27</v>
+      </c>
+      <c r="AI4" s="33">
+        <v>28</v>
+      </c>
+      <c r="AJ4" s="33">
+        <v>29</v>
+      </c>
+      <c r="AK4" s="33">
+        <v>30</v>
+      </c>
+      <c r="AL4" s="33">
+        <v>31</v>
+      </c>
+      <c r="AM4" s="33">
+        <v>32</v>
+      </c>
+      <c r="AN4" s="33">
+        <v>33</v>
+      </c>
+      <c r="AO4" s="33">
+        <v>34</v>
+      </c>
+      <c r="AP4" s="33">
+        <v>35</v>
+      </c>
+      <c r="AQ4" s="33">
+        <v>36</v>
+      </c>
+      <c r="AR4" s="33">
+        <v>37</v>
+      </c>
+      <c r="AS4" s="33">
+        <v>38</v>
+      </c>
+      <c r="AT4" s="33">
+        <v>39</v>
+      </c>
+      <c r="AU4" s="33">
+        <v>40</v>
+      </c>
+      <c r="AV4" s="33">
+        <v>41</v>
+      </c>
+      <c r="AW4" s="33">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8">
+        <v>6</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8">
+        <v>6</v>
+      </c>
+      <c r="G5" s="35">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
+      <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
+      <c r="AW5" s="5"/>
+    </row>
+    <row r="6" spans="1:49" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
         <v>4</v>
       </c>
-      <c r="H2" s="13">
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
+        <v>4</v>
+      </c>
+      <c r="G6" s="35">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="5"/>
+      <c r="AQ6" s="5"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="5"/>
+      <c r="AT6" s="5"/>
+      <c r="AU6" s="5"/>
+      <c r="AV6" s="5"/>
+      <c r="AW6" s="5"/>
+    </row>
+    <row r="7" spans="1:49" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="8">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8">
+        <v>33</v>
+      </c>
+      <c r="E7" s="8">
+        <v>4</v>
+      </c>
+      <c r="F7" s="8">
+        <v>33</v>
+      </c>
+      <c r="G7" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="5"/>
+      <c r="AQ7" s="5"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="5"/>
+      <c r="AU7" s="5"/>
+      <c r="AV7" s="5"/>
+      <c r="AW7" s="5"/>
+    </row>
+    <row r="8" spans="1:49" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8">
+        <v>4</v>
+      </c>
+      <c r="E8" s="8">
+        <v>4</v>
+      </c>
+      <c r="F8" s="8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="35">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="5"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="5"/>
+      <c r="AJ8" s="5"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="5"/>
+      <c r="AM8" s="5"/>
+      <c r="AN8" s="5"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="5"/>
+      <c r="AQ8" s="5"/>
+      <c r="AR8" s="5"/>
+      <c r="AS8" s="5"/>
+      <c r="AT8" s="5"/>
+      <c r="AU8" s="5"/>
+      <c r="AV8" s="5"/>
+      <c r="AW8" s="5"/>
+    </row>
+    <row r="9" spans="1:49" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="8">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2</v>
+      </c>
+      <c r="E9" s="8">
+        <v>4</v>
+      </c>
+      <c r="F9" s="8">
+        <v>2</v>
+      </c>
+      <c r="G9" s="35">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="5"/>
+      <c r="AF9" s="5"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="5"/>
+      <c r="AI9" s="5"/>
+      <c r="AJ9" s="5"/>
+      <c r="AK9" s="5"/>
+      <c r="AL9" s="5"/>
+      <c r="AM9" s="5"/>
+      <c r="AN9" s="5"/>
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="5"/>
+      <c r="AQ9" s="5"/>
+      <c r="AR9" s="5"/>
+      <c r="AS9" s="5"/>
+      <c r="AT9" s="5"/>
+      <c r="AU9" s="5"/>
+      <c r="AV9" s="5"/>
+      <c r="AW9" s="5"/>
+    </row>
+    <row r="10" spans="1:49" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="8">
+        <v>4</v>
+      </c>
+      <c r="D10" s="8">
+        <v>10</v>
+      </c>
+      <c r="E10" s="8">
+        <v>4</v>
+      </c>
+      <c r="F10" s="8">
+        <v>10</v>
+      </c>
+      <c r="G10" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="5"/>
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="5"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="5"/>
+      <c r="AQ10" s="5"/>
+      <c r="AR10" s="5"/>
+      <c r="AS10" s="5"/>
+      <c r="AT10" s="5"/>
+      <c r="AU10" s="5"/>
+      <c r="AV10" s="5"/>
+      <c r="AW10" s="5"/>
+    </row>
+    <row r="11" spans="1:49" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="8">
+        <v>4</v>
+      </c>
+      <c r="D11" s="8">
+        <v>3</v>
+      </c>
+      <c r="E11" s="8">
+        <v>4</v>
+      </c>
+      <c r="F11" s="8">
+        <v>3</v>
+      </c>
+      <c r="G11" s="35">
+        <v>1</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="5"/>
+      <c r="AI11" s="5"/>
+      <c r="AJ11" s="5"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="5"/>
+      <c r="AM11" s="5"/>
+      <c r="AN11" s="5"/>
+      <c r="AO11" s="5"/>
+      <c r="AP11" s="5"/>
+      <c r="AQ11" s="5"/>
+      <c r="AR11" s="5"/>
+      <c r="AS11" s="5"/>
+      <c r="AT11" s="5"/>
+      <c r="AU11" s="5"/>
+      <c r="AV11" s="5"/>
+      <c r="AW11" s="5"/>
+    </row>
+    <row r="12" spans="1:49" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="8">
+        <v>9</v>
+      </c>
+      <c r="D12" s="8">
+        <v>33</v>
+      </c>
+      <c r="E12" s="8">
+        <v>9</v>
+      </c>
+      <c r="F12" s="8">
+        <v>33</v>
+      </c>
+      <c r="G12" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="5"/>
+      <c r="AF12" s="5"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="5"/>
+      <c r="AI12" s="5"/>
+      <c r="AJ12" s="5"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="5"/>
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="5"/>
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="5"/>
+      <c r="AQ12" s="5"/>
+      <c r="AR12" s="5"/>
+      <c r="AS12" s="5"/>
+      <c r="AT12" s="5"/>
+      <c r="AU12" s="5"/>
+      <c r="AV12" s="5"/>
+      <c r="AW12" s="5"/>
+    </row>
+    <row r="13" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="35"/>
-      <c r="AH2" s="18"/>
-      <c r="AI2" s="20" t="s">
+      <c r="B13" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="8">
+        <v>8</v>
+      </c>
+      <c r="D13" s="8">
+        <v>11</v>
+      </c>
+      <c r="E13" s="8">
+        <v>8</v>
+      </c>
+      <c r="F13" s="8">
+        <v>7</v>
+      </c>
+      <c r="G13" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="5"/>
+      <c r="AI13" s="5"/>
+      <c r="AJ13" s="5"/>
+      <c r="AK13" s="5"/>
+      <c r="AL13" s="5"/>
+      <c r="AM13" s="5"/>
+      <c r="AN13" s="5"/>
+      <c r="AO13" s="5"/>
+      <c r="AP13" s="5"/>
+      <c r="AQ13" s="5"/>
+      <c r="AR13" s="5"/>
+      <c r="AS13" s="5"/>
+      <c r="AT13" s="5"/>
+      <c r="AU13" s="5"/>
+      <c r="AV13" s="5"/>
+      <c r="AW13" s="5"/>
+    </row>
+    <row r="14" spans="1:49" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="8">
+        <v>19</v>
+      </c>
+      <c r="D14" s="8">
+        <v>13</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="5"/>
+      <c r="AJ14" s="5"/>
+      <c r="AK14" s="5"/>
+      <c r="AL14" s="5"/>
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="5"/>
+      <c r="AO14" s="5"/>
+      <c r="AP14" s="5"/>
+      <c r="AQ14" s="5"/>
+      <c r="AR14" s="5"/>
+      <c r="AS14" s="5"/>
+      <c r="AT14" s="5"/>
+      <c r="AU14" s="5"/>
+      <c r="AV14" s="5"/>
+      <c r="AW14" s="5"/>
+    </row>
+    <row r="15" spans="1:49" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="8">
+        <v>20</v>
+      </c>
+      <c r="D15" s="8">
+        <v>12</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="5"/>
+      <c r="AF15" s="5"/>
+      <c r="AG15" s="5"/>
+      <c r="AH15" s="5"/>
+      <c r="AI15" s="5"/>
+      <c r="AJ15" s="5"/>
+      <c r="AK15" s="5"/>
+      <c r="AL15" s="5"/>
+      <c r="AM15" s="5"/>
+      <c r="AN15" s="5"/>
+      <c r="AO15" s="5"/>
+      <c r="AP15" s="5"/>
+      <c r="AQ15" s="5"/>
+      <c r="AR15" s="5"/>
+      <c r="AS15" s="5"/>
+      <c r="AT15" s="5"/>
+      <c r="AU15" s="5"/>
+      <c r="AV15" s="5"/>
+      <c r="AW15" s="5"/>
+    </row>
+    <row r="16" spans="1:49" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="8">
+        <v>30</v>
+      </c>
+      <c r="D16" s="8">
+        <v>6</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="5"/>
+      <c r="AG16" s="5"/>
+      <c r="AH16" s="5"/>
+      <c r="AI16" s="5"/>
+      <c r="AJ16" s="5"/>
+      <c r="AK16" s="5"/>
+      <c r="AL16" s="5"/>
+      <c r="AM16" s="5"/>
+      <c r="AN16" s="5"/>
+      <c r="AO16" s="5"/>
+      <c r="AP16" s="5"/>
+      <c r="AQ16" s="5"/>
+      <c r="AR16" s="5"/>
+      <c r="AS16" s="5"/>
+      <c r="AT16" s="5"/>
+      <c r="AU16" s="5"/>
+      <c r="AV16" s="5"/>
+      <c r="AW16" s="5"/>
+    </row>
+    <row r="17" spans="1:49" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="8">
+        <v>32</v>
+      </c>
+      <c r="D17" s="8">
         <v>3</v>
       </c>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
-      <c r="AL2" s="21"/>
-      <c r="AM2" s="21"/>
-      <c r="AN2" s="21"/>
-      <c r="AO2" s="21"/>
-      <c r="AP2" s="21"/>
-    </row>
-    <row r="3" spans="2:49" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="25" t="s">
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="5"/>
+      <c r="AH17" s="5"/>
+      <c r="AI17" s="5"/>
+      <c r="AJ17" s="5"/>
+      <c r="AK17" s="5"/>
+      <c r="AL17" s="5"/>
+      <c r="AM17" s="5"/>
+      <c r="AN17" s="5"/>
+      <c r="AO17" s="5"/>
+      <c r="AP17" s="5"/>
+      <c r="AQ17" s="5"/>
+      <c r="AR17" s="5"/>
+      <c r="AS17" s="5"/>
+      <c r="AT17" s="5"/>
+      <c r="AU17" s="5"/>
+      <c r="AV17" s="5"/>
+      <c r="AW17" s="5"/>
+    </row>
+    <row r="18" spans="1:49" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="37">
+        <v>31</v>
+      </c>
+      <c r="D18" s="8">
         <v>6</v>
       </c>
-      <c r="E3" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AC3" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ3" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ3" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="3">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3">
-        <v>2</v>
-      </c>
-      <c r="J4" s="3">
-        <v>3</v>
-      </c>
-      <c r="K4" s="3">
-        <v>4</v>
-      </c>
-      <c r="L4" s="3">
-        <v>5</v>
-      </c>
-      <c r="M4" s="3">
-        <v>6</v>
-      </c>
-      <c r="N4" s="3">
-        <v>7</v>
-      </c>
-      <c r="O4" s="3">
-        <v>8</v>
-      </c>
-      <c r="P4" s="3">
-        <v>9</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>10</v>
-      </c>
-      <c r="R4" s="3">
-        <v>11</v>
-      </c>
-      <c r="S4" s="3">
-        <v>12</v>
-      </c>
-      <c r="T4" s="3">
-        <v>13</v>
-      </c>
-      <c r="U4" s="3">
-        <v>14</v>
-      </c>
-      <c r="V4" s="3">
-        <v>15</v>
-      </c>
-      <c r="W4" s="3">
-        <v>16</v>
-      </c>
-      <c r="X4" s="3">
-        <v>17</v>
-      </c>
-      <c r="Y4" s="3">
-        <v>18</v>
-      </c>
-      <c r="Z4" s="3">
-        <v>19</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>20</v>
-      </c>
-      <c r="AB4" s="3">
-        <v>21</v>
-      </c>
-      <c r="AC4" s="3">
-        <v>22</v>
-      </c>
-      <c r="AD4" s="3">
-        <v>23</v>
-      </c>
-      <c r="AE4" s="3">
-        <v>24</v>
-      </c>
-      <c r="AF4" s="3">
-        <v>25</v>
-      </c>
-      <c r="AG4" s="3">
-        <v>26</v>
-      </c>
-      <c r="AH4" s="3">
-        <v>27</v>
-      </c>
-      <c r="AI4" s="3">
-        <v>28</v>
-      </c>
-      <c r="AJ4" s="3">
-        <v>29</v>
-      </c>
-      <c r="AK4" s="3">
-        <v>30</v>
-      </c>
-      <c r="AL4" s="3">
-        <v>31</v>
-      </c>
-      <c r="AM4" s="3">
-        <v>32</v>
-      </c>
-      <c r="AN4" s="3">
-        <v>33</v>
-      </c>
-      <c r="AO4" s="3">
-        <v>34</v>
-      </c>
-      <c r="AP4" s="3">
-        <v>35</v>
-      </c>
-      <c r="AQ4" s="3">
-        <v>36</v>
-      </c>
-      <c r="AR4" s="3">
-        <v>37</v>
-      </c>
-      <c r="AS4" s="3">
-        <v>38</v>
-      </c>
-      <c r="AT4" s="3">
-        <v>39</v>
-      </c>
-      <c r="AU4" s="3">
-        <v>40</v>
-      </c>
-      <c r="AV4" s="3">
-        <v>41</v>
-      </c>
-      <c r="AW4" s="3">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="2:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6">
-        <v>6</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6">
-        <v>6</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="6">
-        <v>4</v>
-      </c>
-      <c r="G6" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="6">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6">
-        <v>33</v>
-      </c>
-      <c r="E7" s="6">
-        <v>4</v>
-      </c>
-      <c r="F7" s="6">
-        <v>33</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="8" spans="2:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="6">
-        <v>4</v>
-      </c>
-      <c r="D8" s="6">
-        <v>4</v>
-      </c>
-      <c r="E8" s="6">
-        <v>4</v>
-      </c>
-      <c r="F8" s="6">
-        <v>4</v>
-      </c>
-      <c r="G8" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="6">
-        <v>4</v>
-      </c>
-      <c r="D9" s="6">
-        <v>2</v>
-      </c>
-      <c r="E9" s="6">
-        <v>4</v>
-      </c>
-      <c r="F9" s="6">
-        <v>2</v>
-      </c>
-      <c r="G9" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="6">
-        <v>4</v>
-      </c>
-      <c r="D10" s="6">
-        <v>10</v>
-      </c>
-      <c r="E10" s="6">
-        <v>4</v>
-      </c>
-      <c r="F10" s="6">
-        <v>10</v>
-      </c>
-      <c r="G10" s="7">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="6">
-        <v>4</v>
-      </c>
-      <c r="D11" s="6">
-        <v>3</v>
-      </c>
-      <c r="E11" s="6">
-        <v>4</v>
-      </c>
-      <c r="F11" s="6">
-        <v>3</v>
-      </c>
-      <c r="G11" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="6">
-        <v>8</v>
-      </c>
-      <c r="D12" s="6">
-        <v>11</v>
-      </c>
-      <c r="E12" s="6">
-        <v>8</v>
-      </c>
-      <c r="F12" s="6">
-        <v>7</v>
-      </c>
-      <c r="G12" s="7">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="6">
-        <v>19</v>
-      </c>
-      <c r="D13" s="6">
-        <v>13</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="2:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="6">
-        <v>20</v>
-      </c>
-      <c r="D14" s="6">
-        <v>12</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="2:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="6">
-        <v>30</v>
-      </c>
-      <c r="D15" s="6">
-        <v>6</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="2:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="6">
-        <v>32</v>
-      </c>
-      <c r="D16" s="6">
-        <v>3</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="8">
-        <v>31</v>
-      </c>
-      <c r="D17" s="6">
-        <v>6</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-      <c r="O18"/>
-      <c r="P18"/>
-      <c r="Q18"/>
-      <c r="R18"/>
-      <c r="S18"/>
-      <c r="T18"/>
-      <c r="U18"/>
-      <c r="V18"/>
-      <c r="W18"/>
-      <c r="X18"/>
-      <c r="Y18"/>
-      <c r="Z18"/>
-      <c r="AA18"/>
-    </row>
-    <row r="19" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="5"/>
+      <c r="AG18" s="5"/>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="5"/>
+      <c r="AJ18" s="5"/>
+      <c r="AK18" s="5"/>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="5"/>
+      <c r="AN18" s="5"/>
+      <c r="AO18" s="5"/>
+      <c r="AP18" s="5"/>
+      <c r="AQ18" s="5"/>
+      <c r="AR18" s="5"/>
+      <c r="AS18" s="5"/>
+      <c r="AT18" s="5"/>
+      <c r="AU18" s="5"/>
+      <c r="AV18" s="5"/>
+      <c r="AW18" s="5"/>
+    </row>
+    <row r="19" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
@@ -1623,7 +2249,7 @@
       <c r="Z19"/>
       <c r="AA19"/>
     </row>
-    <row r="20" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
@@ -1651,7 +2277,7 @@
       <c r="Z20"/>
       <c r="AA20"/>
     </row>
-    <row r="21" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
@@ -1679,7 +2305,7 @@
       <c r="Z21"/>
       <c r="AA21"/>
     </row>
-    <row r="22" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
@@ -1707,7 +2333,7 @@
       <c r="Z22"/>
       <c r="AA22"/>
     </row>
-    <row r="23" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
@@ -1735,7 +2361,7 @@
       <c r="Z23"/>
       <c r="AA23"/>
     </row>
-    <row r="24" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
@@ -1763,7 +2389,7 @@
       <c r="Z24"/>
       <c r="AA24"/>
     </row>
-    <row r="25" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
@@ -1791,7 +2417,7 @@
       <c r="Z25"/>
       <c r="AA25"/>
     </row>
-    <row r="26" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
@@ -1819,7 +2445,7 @@
       <c r="Z26"/>
       <c r="AA26"/>
     </row>
-    <row r="27" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
@@ -1847,7 +2473,7 @@
       <c r="Z27"/>
       <c r="AA27"/>
     </row>
-    <row r="28" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
@@ -1875,7 +2501,7 @@
       <c r="Z28"/>
       <c r="AA28"/>
     </row>
-    <row r="29" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -1903,7 +2529,7 @@
       <c r="Z29"/>
       <c r="AA29"/>
     </row>
-    <row r="30" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
@@ -1931,7 +2557,7 @@
       <c r="Z30"/>
       <c r="AA30"/>
     </row>
-    <row r="31" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
@@ -1959,7 +2585,7 @@
       <c r="Z31"/>
       <c r="AA31"/>
     </row>
-    <row r="32" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
@@ -1987,6 +2613,34 @@
       <c r="Z32"/>
       <c r="AA32"/>
     </row>
+    <row r="33" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+      <c r="Z33"/>
+      <c r="AA33"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="AI2:AP2"/>
@@ -2002,7 +2656,7 @@
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:AW17">
+  <conditionalFormatting sqref="H5:AW18">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -2028,7 +2682,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33:BO33">
+  <conditionalFormatting sqref="AX33:BO33 B34:AW34">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>